<commit_message>
added pump for pressurization of input to dehydration reaction
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/HP/analyses/0_baseline.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/HP/analyses/0_baseline.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Biorefinery</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Adjusted product yield [10^6 kg/yr]</t>
   </si>
   <si>
+    <t>Product recovery [%]</t>
+  </si>
+  <si>
     <t>Total capital investment [10^6 $]</t>
   </si>
   <si>
@@ -94,30 +97,48 @@
     <t>feedstock [10^6 $/yr]</t>
   </si>
   <si>
+    <t>sulfuric_acid_fresh [10^6 $/yr]</t>
+  </si>
+  <si>
     <t>enzyme [10^6 $/yr]</t>
   </si>
   <si>
     <t>boiler_chems [10^6 $/yr]</t>
   </si>
   <si>
+    <t>sulfuric_acid_fresh2 [10^6 $/yr]</t>
+  </si>
+  <si>
     <t>baghouse_bag [10^6 $/yr]</t>
   </si>
   <si>
-    <t>lime [10^6 $/yr]</t>
+    <t>ammonia_fresh [10^6 $/yr]</t>
   </si>
   <si>
     <t>natural_gas [10^6 $/yr]</t>
   </si>
   <si>
+    <t>CSL_fresh [10^6 $/yr]</t>
+  </si>
+  <si>
     <t>cooling_tower_chems [10^6 $/yr]</t>
   </si>
   <si>
-    <t>CSL_fresh [10^6 $/yr]</t>
-  </si>
-  <si>
     <t>lime_fresh [10^6 $/yr]</t>
   </si>
   <si>
+    <t>hexanol_fresh [10^6 $/yr]</t>
+  </si>
+  <si>
+    <t>aerobic_caustic [10^6 $/yr]</t>
+  </si>
+  <si>
+    <t>TOA_fresh [10^6 $/yr]</t>
+  </si>
+  <si>
+    <t>AQ336_fresh [10^6 $/yr]</t>
+  </si>
+  <si>
     <t>system_makeup_water [10^6 $/yr]</t>
   </si>
   <si>
@@ -127,12 +148,12 @@
     <t>Check [10^6 $/yr]</t>
   </si>
   <si>
+    <t>AcrylicAcid [10^6 $/yr]</t>
+  </si>
+  <si>
     <t>ash [10^6 $/yr]</t>
   </si>
   <si>
-    <t>AcrylicAcid [10^6 $/yr]</t>
-  </si>
-  <si>
     <t>gypsum [10^6 $/yr]</t>
   </si>
   <si>
@@ -161,6 +182,9 @@
   </si>
   <si>
     <t>Net present value [$]</t>
+  </si>
+  <si>
+    <t>HXN energy balance error</t>
   </si>
   <si>
     <t>initial</t>
@@ -524,13 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:BB5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:46">
+    <row r="1" spans="1:54">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -549,13 +573,13 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -566,37 +590,47 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AK1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1" t="s">
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1" t="s">
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="BB1" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:54">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -692,337 +726,391 @@
         <v>39</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AK2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AL2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="AO2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AP2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>48</v>
+      <c r="BA2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BB2" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:54">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B4">
-        <v>1.126227815542428</v>
+        <v>1.444711401387989</v>
       </c>
       <c r="C4">
-        <v>0.03125775636197925</v>
+        <v>0.01839700388503976</v>
       </c>
       <c r="D4">
-        <v>0.9623817774825738</v>
+        <v>0.9372059240906464</v>
       </c>
       <c r="E4">
-        <v>1.170250565856955</v>
+        <v>1.541509011224655</v>
       </c>
       <c r="F4">
-        <v>0.03008189512775882</v>
+        <v>0.0172417810265779</v>
       </c>
       <c r="G4">
-        <v>694.696429143707</v>
+        <v>0.04894712477631048</v>
       </c>
       <c r="H4">
-        <v>177.3688482654326</v>
+        <v>550.4327117045649</v>
       </c>
       <c r="I4">
-        <v>146.4580599519613</v>
+        <v>136.0671414320992</v>
       </c>
       <c r="J4">
-        <v>264.797132622219</v>
+        <v>139.6488449785993</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>205.2578208430793</v>
       </c>
       <c r="L4">
-        <v>99.26177252129467</v>
+        <v>0.004346704959358991</v>
       </c>
       <c r="M4">
-        <v>49.76917528525546</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>595.3255770855873</v>
+        <v>132.9079607470987</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>527.4753828601263</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>-363.8516315211003</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>0.01151669545834485</v>
+        <v>-300.05251655464</v>
       </c>
       <c r="S4">
-        <v>0.0005000012500004999</v>
+        <v>0.006547536261</v>
       </c>
       <c r="T4">
-        <v>1.672709323760401E-06</v>
+        <v>0.0001877794398684067</v>
       </c>
       <c r="U4">
-        <v>1.149218560638985E-05</v>
+        <v>0.003543296856379546</v>
       </c>
       <c r="V4">
-        <v>2.5666730833359E-05</v>
+        <v>1.287278670316298E-06</v>
       </c>
       <c r="W4">
-        <v>0.0005977492985121309</v>
+        <v>0.001674664502029958</v>
       </c>
       <c r="X4">
-        <v>1.011999582962241E-05</v>
+        <v>8.844122045762369E-06</v>
       </c>
       <c r="Y4">
-        <v>9.953849461038739E-05</v>
+        <v>0.0002947832196165155</v>
       </c>
       <c r="Z4">
-        <v>0.005188225206352423</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>1.454293883396211E-05</v>
+        <v>0.0002772757791182015</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>1.279689809364887E-05</v>
       </c>
       <c r="AC4">
-        <v>-146.4394833334996</v>
+        <v>0.003156830072960897</v>
       </c>
       <c r="AD4">
-        <v>-0.0008083534109588949</v>
+        <v>0.000647873592065376</v>
       </c>
       <c r="AE4">
-        <v>0.03520335479530935</v>
+        <v>0.001319431938122132</v>
       </c>
       <c r="AF4">
         <v>0</v>
       </c>
       <c r="AG4">
-        <v>-264.7635459742456</v>
+        <v>0</v>
       </c>
       <c r="AH4">
-        <v>0</v>
+        <v>3.041193949065498E-05</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>0.992584721474037</v>
       </c>
       <c r="AJ4">
-        <v>0.6263736590069705</v>
+        <v>-139.6311320352991</v>
       </c>
       <c r="AK4">
-        <v>0</v>
+        <v>0.02657836082203212</v>
       </c>
       <c r="AL4">
-        <v>0</v>
+        <v>-0.0002718148070663304</v>
       </c>
       <c r="AM4">
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>-0.5242375815974929</v>
+        <v>-205.2317861118714</v>
       </c>
       <c r="AO4">
         <v>0</v>
       </c>
       <c r="AP4">
-        <v>18921.37618158883</v>
+        <v>0</v>
       </c>
       <c r="AQ4">
-        <v>-18921.37618158883</v>
+        <v>0.4820427790017772</v>
       </c>
       <c r="AR4">
-        <v>10.44232908709525</v>
+        <v>0.1832166884283716</v>
       </c>
       <c r="AS4">
-        <v>-10.44232908709525</v>
+        <v>0</v>
       </c>
       <c r="AT4">
-        <v>0.05681265704333782</v>
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>-0.6629068846972399</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>-32770.74806031636</v>
+      </c>
+      <c r="AX4">
+        <v>32770.74806031636</v>
+      </c>
+      <c r="AY4">
+        <v>-18.0855204395274</v>
+      </c>
+      <c r="AZ4">
+        <v>18.0855204395274</v>
+      </c>
+      <c r="BA4">
+        <v>-0.1941508809104562</v>
+      </c>
+      <c r="BB4">
+        <v>-13.38891330346364</v>
       </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:54">
       <c r="A5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>1.113100988926977</v>
+        <v>58</v>
       </c>
       <c r="C5">
-        <v>0.03125898942567343</v>
+        <v>0.01838647561858705</v>
       </c>
       <c r="D5">
-        <v>0.962381777516679</v>
-      </c>
-      <c r="E5">
-        <v>1.156610468490506</v>
+        <v>0.9372059244716893</v>
       </c>
       <c r="F5">
-        <v>0.03008308180685466</v>
+        <v>0.01723191387989405</v>
       </c>
       <c r="G5">
-        <v>670.0911749912674</v>
+        <v>0.04894651852624667</v>
       </c>
       <c r="H5">
-        <v>177.1393488372352</v>
+        <v>264.4943313167407</v>
       </c>
       <c r="I5">
-        <v>146.4599695231909</v>
+        <v>132.6968091273906</v>
       </c>
       <c r="J5">
-        <v>261.5728583366641</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
+        <v>139.6344753134799</v>
       </c>
       <c r="L5">
-        <v>99.26177253510183</v>
+        <v>0.00434771713824285</v>
       </c>
       <c r="M5">
-        <v>49.76918049580499</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>595.3305223267615</v>
+        <v>132.9076343377146</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>527.3340934861478</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>-349.6001385644735</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>0.01151669545834485</v>
+        <v>-138.2560409154121</v>
       </c>
       <c r="S5">
-        <v>0.0005000012500004999</v>
+        <v>0.006547536261</v>
       </c>
       <c r="T5">
-        <v>1.672720912238352E-06</v>
+        <v>0.0001877794398684067</v>
       </c>
       <c r="U5">
-        <v>1.14922652238928E-05</v>
+        <v>0.003543296856379546</v>
       </c>
       <c r="V5">
-        <v>2.5666730833359E-05</v>
+        <v>1.287215242436646E-06</v>
       </c>
       <c r="W5">
-        <v>0.0005977754517736613</v>
+        <v>0.001674146510928734</v>
       </c>
       <c r="X5">
-        <v>1.012030226091494E-05</v>
+        <v>8.84368627072649E-06</v>
       </c>
       <c r="Y5">
-        <v>9.953896604229527E-05</v>
+        <v>0.0002947832196165155</v>
       </c>
       <c r="Z5">
-        <v>0.005188413825226751</v>
+        <v>0</v>
       </c>
       <c r="AA5">
-        <v>1.454326158728984E-05</v>
+        <v>0.0002772636918950845</v>
       </c>
       <c r="AB5">
-        <v>1</v>
+        <v>1.279360945898322E-05</v>
       </c>
       <c r="AC5">
-        <v>-146.4413926625208</v>
+        <v>0.003155914920121179</v>
       </c>
       <c r="AD5">
-        <v>-0.0008083618182235248</v>
+        <v>0.0006475348415891196</v>
       </c>
       <c r="AE5">
-        <v>0.0347944073422644</v>
+        <v>0.001319389963286179</v>
       </c>
       <c r="AF5">
         <v>0</v>
       </c>
       <c r="AG5">
-        <v>-261.5396806529582</v>
+        <v>0</v>
       </c>
       <c r="AH5">
-        <v>0</v>
+        <v>3.041954664016514E-05</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>0.9925824822518037</v>
       </c>
       <c r="AJ5">
-        <v>0.6263779985041165</v>
-      </c>
-      <c r="AK5">
-        <v>0</v>
+        <v>-139.6167641928161</v>
       </c>
       <c r="AL5">
-        <v>0</v>
+        <v>-0.000271791687012924</v>
       </c>
       <c r="AM5">
         <v>0</v>
       </c>
-      <c r="AN5">
-        <v>-0.5242534553984732</v>
-      </c>
       <c r="AO5">
         <v>0</v>
       </c>
       <c r="AP5">
-        <v>18921.8349219195</v>
+        <v>0</v>
       </c>
       <c r="AQ5">
-        <v>-18921.8349219195</v>
+        <v>0.482019027383671</v>
       </c>
       <c r="AR5">
-        <v>10.44258225670894</v>
+        <v>0.1832166884204061</v>
       </c>
       <c r="AS5">
-        <v>-10.44258225670894</v>
+        <v>0</v>
       </c>
       <c r="AT5">
-        <v>-2.047668638639152</v>
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>-0.6627365263381156</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>-32786.80172685236</v>
+      </c>
+      <c r="AX5">
+        <v>32786.80172685236</v>
+      </c>
+      <c r="AY5">
+        <v>-18.09438013701528</v>
+      </c>
+      <c r="AZ5">
+        <v>18.09438013701528</v>
+      </c>
+      <c r="BB5">
+        <v>-13.38295943497001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="R1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="S1:AJ1"/>
+    <mergeCell ref="AK1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>